<commit_message>
Added page view and page transitons handling.
</commit_message>
<xml_diff>
--- a/appmodel/pexpress.xlsx
+++ b/appmodel/pexpress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/navendusinha/PycharmProjects/neoWebUI/appmodel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E633DFB5-2F4E-8D49-9F69-9BED005ED8BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF97B28-DC0A-5846-894B-11CD0845A2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="2220" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{B230B229-1191-BA4F-B757-C9FE5A580652}"/>
+    <workbookView xWindow="1900" yWindow="2220" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{B230B229-1191-BA4F-B757-C9FE5A580652}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="2" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="62">
   <si>
     <t>Appname</t>
   </si>
@@ -178,9 +178,6 @@
   </si>
   <si>
     <t>userid</t>
-  </si>
-  <si>
-    <t>prequest</t>
   </si>
   <si>
     <t>TabView</t>
@@ -824,7 +821,7 @@
   <dimension ref="B1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="B1" sqref="B1:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -935,41 +932,41 @@
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s">
         <v>44</v>
-      </c>
-      <c r="C9" t="s">
-        <v>45</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E10" s="16">
         <v>10000</v>
@@ -977,16 +974,16 @@
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" t="s">
         <v>48</v>
-      </c>
-      <c r="C11" t="s">
-        <v>49</v>
       </c>
       <c r="D11" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
@@ -1007,8 +1004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27B0635B-1A6B-4E4D-B464-016C4F031864}">
   <dimension ref="B1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1031,10 +1028,10 @@
         <v>36</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
@@ -1043,16 +1040,16 @@
         <v>signup</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
         <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
@@ -1063,13 +1060,13 @@
         <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
@@ -1080,13 +1077,13 @@
         <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
@@ -1097,13 +1094,13 @@
         <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
@@ -1114,13 +1111,13 @@
         <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
@@ -1138,8 +1135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{059BCA2A-83EF-7F41-BA79-DE47A930F44C}">
   <dimension ref="B1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1150,13 +1147,13 @@
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
         <v>59</v>
-      </c>
-      <c r="D1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
@@ -1165,7 +1162,7 @@
         <v>LoginRegister</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
@@ -1173,7 +1170,7 @@
         <v>AppLoad</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
@@ -1206,7 +1203,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D1" s="12"/>
     </row>

</xml_diff>

<commit_message>
Added YAML model parser and handler
</commit_message>
<xml_diff>
--- a/appmodel/pexpress.xlsx
+++ b/appmodel/pexpress.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/navendusinha/PycharmProjects/neoWebUI/appmodel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF97B28-DC0A-5846-894B-11CD0845A2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72724E29-03A5-4647-8F4B-0ED06AB9EB4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="2220" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{B230B229-1191-BA4F-B757-C9FE5A580652}"/>
+    <workbookView xWindow="1380" yWindow="840" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{B230B229-1191-BA4F-B757-C9FE5A580652}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="2" r:id="rId1"/>
-    <sheet name="Forms" sheetId="1" r:id="rId2"/>
-    <sheet name="Backend" sheetId="4" r:id="rId3"/>
-    <sheet name="PageViews" sheetId="7" r:id="rId4"/>
-    <sheet name="FormViews" sheetId="6" r:id="rId5"/>
-    <sheet name="Queries" sheetId="5" r:id="rId6"/>
-    <sheet name="Layout" sheetId="3" r:id="rId7"/>
+    <sheet name="Views" sheetId="8" r:id="rId2"/>
+    <sheet name="Forms" sheetId="1" r:id="rId3"/>
+    <sheet name="Backend" sheetId="4" r:id="rId4"/>
+    <sheet name="PageViews" sheetId="7" r:id="rId5"/>
+    <sheet name="FormViews" sheetId="6" r:id="rId6"/>
+    <sheet name="Queries" sheetId="5" r:id="rId7"/>
+    <sheet name="Layout" sheetId="3" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="74">
   <si>
     <t>Appname</t>
   </si>
@@ -228,9 +229,6 @@
     <t>Portfolio</t>
   </si>
   <si>
-    <t>PNews</t>
-  </si>
-  <si>
     <t>PageView</t>
   </si>
   <si>
@@ -250,6 +248,45 @@
   </si>
   <si>
     <t>callback:signin</t>
+  </si>
+  <si>
+    <t>News</t>
+  </si>
+  <si>
+    <t>View</t>
+  </si>
+  <si>
+    <t>Widget</t>
+  </si>
+  <si>
+    <t>container</t>
+  </si>
+  <si>
+    <t>This is a cool news feed</t>
+  </si>
+  <si>
+    <t>newsid</t>
+  </si>
+  <si>
+    <t>loadnews</t>
+  </si>
+  <si>
+    <t>BackendAPI</t>
+  </si>
+  <si>
+    <t>Visitors</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>vistors</t>
+  </si>
+  <si>
+    <t>getvisitors</t>
+  </si>
+  <si>
+    <t>This is a table content for visitors</t>
   </si>
 </sst>
 </file>
@@ -463,15 +500,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -817,11 +854,100 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6BFEE84-0CAA-4542-9700-FDC9EC1E6DB7}">
+  <dimension ref="B1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="17.83203125" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F7" s="1"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F10" s="15"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F12" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" display="johndoe@email.com" xr:uid="{D73E4CD1-EC1D-AC45-89B0-AC154DDF122A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEC91076-B794-D24C-81D3-BD11A24F9ACB}">
   <dimension ref="B1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -848,30 +974,30 @@
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
@@ -879,13 +1005,13 @@
         <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
@@ -893,18 +1019,18 @@
         <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>35</v>
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
         <v>37</v>
@@ -916,9 +1042,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
         <v>35</v>
@@ -926,7 +1052,7 @@
       <c r="D7" t="s">
         <v>35</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>35</v>
       </c>
     </row>
@@ -968,7 +1094,7 @@
       <c r="D10" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="15">
         <v>10000</v>
       </c>
     </row>
@@ -992,20 +1118,20 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E5" r:id="rId1" display="johndoe@email.com" xr:uid="{5D92B118-9E6F-3A4F-BD5E-609150A1352B}"/>
-    <hyperlink ref="E6" r:id="rId2" xr:uid="{D65AD12B-2157-B548-B8F7-6D3CD4F58E1D}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{FE7300D1-33D2-3248-9DB9-F081C6B15198}"/>
+    <hyperlink ref="E7" r:id="rId1" display="johndoe@email.com" xr:uid="{5D92B118-9E6F-3A4F-BD5E-609150A1352B}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{D65AD12B-2157-B548-B8F7-6D3CD4F58E1D}"/>
+    <hyperlink ref="E6" r:id="rId3" xr:uid="{FE7300D1-33D2-3248-9DB9-F081C6B15198}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27B0635B-1A6B-4E4D-B464-016C4F031864}">
   <dimension ref="B1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1018,55 +1144,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>28</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="20" t="s">
-        <v>55</v>
+      <c r="F1" s="19" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" t="str" cm="1">
         <f t="array" ref="B2:B7">_xlfn.UNIQUE(Forms!B2:B93)</f>
-        <v>signup</v>
+        <v>signin</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
         <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" t="str">
-        <v>signin</v>
+        <v>signup</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
         <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
@@ -1083,7 +1209,7 @@
         <v>52</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
@@ -1100,7 +1226,7 @@
         <v>53</v>
       </c>
       <c r="F5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
@@ -1114,10 +1240,10 @@
         <v>47</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="F6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
@@ -1131,7 +1257,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{059BCA2A-83EF-7F41-BA79-DE47A930F44C}">
   <dimension ref="B1:D4"/>
   <sheetViews>
@@ -1146,14 +1272,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B1" s="21" t="s">
-        <v>55</v>
+      <c r="B1" s="20" t="s">
+        <v>54</v>
       </c>
       <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
         <v>58</v>
-      </c>
-      <c r="D1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
@@ -1162,7 +1288,7 @@
         <v>LoginRegister</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
@@ -1170,7 +1296,7 @@
         <v>AppLoad</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
@@ -1183,12 +1309,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28482AD0-F663-164D-B492-E8DD42487F91}">
-  <dimension ref="B1:D7"/>
+  <dimension ref="B1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1209,7 +1335,7 @@
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" t="str" cm="1">
-        <f t="array" ref="B2:B7">_xlfn.UNIQUE(Forms!B2:B93)</f>
+        <f t="array" ref="B2:B6">_xlfn.UNIQUE(Forms!B4:B93)</f>
         <v>signup</v>
       </c>
       <c r="C2" t="s">
@@ -1218,7 +1344,7 @@
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" t="str">
-        <v>signin</v>
+        <v>stocktickers</v>
       </c>
       <c r="C3" t="s">
         <v>27</v>
@@ -1226,7 +1352,7 @@
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" t="str">
-        <v>stocktickers</v>
+        <v>portfolio</v>
       </c>
       <c r="C4" t="s">
         <v>24</v>
@@ -1234,16 +1360,11 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" t="str">
-        <v>portfolio</v>
+        <v>pnews</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B6" t="str">
-        <v>pnews</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B7">
+      <c r="B6">
         <v>0</v>
       </c>
     </row>
@@ -1252,7 +1373,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25CEE5AD-978B-C346-AB0D-436CE01C7E14}">
   <dimension ref="B1:E3"/>
   <sheetViews>
@@ -1301,7 +1422,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C04CBEB2-07CA-4D4E-8E98-2CCD11B504C6}">
   <dimension ref="A1:F24"/>
   <sheetViews>
@@ -1335,10 +1456,10 @@
       <c r="C2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="15"/>
+      <c r="E2" s="21"/>
       <c r="F2" s="7" t="s">
         <v>19</v>
       </c>

</xml_diff>